<commit_message>
Something is very weird in software - going to hour 13 and making  jumps of multiple minutes.
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1B00FE-56D7-4C51-8BC6-80E7ABF19C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4AA60C-1018-47A9-A462-8E0CDDE39BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PR-1" sheetId="1" r:id="rId1"/>
-    <sheet name="PR-2" sheetId="3" r:id="rId2"/>
+    <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
+    <sheet name="LED PCB Assembly" sheetId="5" r:id="rId2"/>
+    <sheet name="PR-1" sheetId="1" r:id="rId3"/>
+    <sheet name="PR-2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="200">
   <si>
     <t>Quantity</t>
   </si>
@@ -596,6 +598,45 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/4149/10123800</t>
+  </si>
+  <si>
+    <t>Red SMT LEDs (surface mount)</t>
+  </si>
+  <si>
+    <t>Red SMT LEDs (surface mount, right angle)</t>
+  </si>
+  <si>
+    <t>MOSFETS</t>
+  </si>
+  <si>
+    <t>caps.</t>
+  </si>
+  <si>
+    <t>res.</t>
+  </si>
+  <si>
+    <t>STM32</t>
+  </si>
+  <si>
+    <t>pull-up resistors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector - Male Receptacle </t>
+  </si>
+  <si>
+    <t>buttons</t>
+  </si>
+  <si>
+    <t>buzzer</t>
+  </si>
+  <si>
+    <t>battery</t>
+  </si>
+  <si>
+    <t>battery connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battery management IC stuff </t>
   </si>
 </sst>
 </file>
@@ -739,14 +780,10 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -754,6 +791,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1047,12 +1102,1580 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535EBE7C-EB1B-4F48-8827-B2C8DF8DD54E}">
+  <dimension ref="A1:L104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="35.109375" customWidth="1"/>
+    <col min="7" max="7" width="9" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="13"/>
+    <col min="9" max="9" width="12.109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="35.5546875" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I3" s="14">
+        <f t="shared" ref="I3:I68" si="0">G3*H3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="L3" s="2">
+        <f>SUM(I3:I105)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="I4" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>195</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>196</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>197</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>198</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>199</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I11" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I12" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I13" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I14" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I15" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I16" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I17" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I18" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I19" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I20" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I22" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I23" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I24" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I25" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I26" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I27" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I29" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I31" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I32" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I34" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I35" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I36" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I37" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I38" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I39" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I40" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I41" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I42" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I43" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I44" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I45" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I46" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I47" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I48" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I50" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I51" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I53" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I54" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I55" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I56" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I57" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I58" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I59" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I60" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I61" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I62" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I63" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I64" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I65" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I66" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I67" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I68" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I69" s="14">
+        <f t="shared" ref="I69:I132" si="1">G69*H69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I70" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I71" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I72" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I73" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I74" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I75" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I76" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I77" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I78" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I79" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I80" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I81" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I82" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I83" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I84" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I85" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I86" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I87" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I88" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I89" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I90" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I91" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I92" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I93" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I94" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I95" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I96" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I97" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I98" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I99" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I100" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I101" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I102" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I103" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I104" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F9AC-3655-4B8A-AD78-25E473D1BEC8}">
+  <dimension ref="A1:L104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="35.109375" customWidth="1"/>
+    <col min="7" max="7" width="9" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="13"/>
+    <col min="9" max="9" width="12.109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="35.5546875" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="4"/>
+      <c r="L3" s="2">
+        <f>SUM(I3:I105)</f>
+        <v>12.370000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>11.38</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" ref="I5:I7" si="0">G5*H5</f>
+        <v>11.38</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.24</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>189</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14">
+        <f t="shared" ref="I7:I70" si="1">G8*H8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>190</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>191</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I11" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I12" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I13" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I14" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I15" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I16" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I17" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I18" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I19" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I20" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I21" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I22" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I23" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I24" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I25" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I26" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I27" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I28" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I29" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I30" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I31" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I32" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I33" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I34" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I35" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I36" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I37" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I38" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I39" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I40" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I41" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I42" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I43" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I44" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I45" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I46" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I47" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I48" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I50" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I51" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I53" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I54" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I55" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I56" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I57" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I58" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I59" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I60" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I61" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I62" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I63" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I64" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I65" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I66" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I67" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I68" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I69" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I70" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I71" s="14">
+        <f t="shared" ref="I71:I104" si="2">G71*H71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I72" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I73" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I74" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I75" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I76" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I77" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I78" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I79" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I80" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I81" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I82" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I83" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I84" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I85" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I86" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I87" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I88" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I89" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I90" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I91" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I92" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I93" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I94" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I95" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I96" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I97" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I98" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I99" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I100" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I101" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I102" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I103" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I104" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J5" r:id="rId1" xr:uid="{6CAFF770-2D29-4F0D-A99E-4F828E77668E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,58 +2684,58 @@
     <col min="2" max="2" width="32.88671875" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="11" customWidth="1"/>
     <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="3"/>
-    <col min="9" max="9" width="17.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="13"/>
+    <col min="9" max="9" width="13.109375" style="13" customWidth="1"/>
     <col min="10" max="10" width="35.5546875" customWidth="1"/>
     <col min="12" max="12" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="10" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1126,26 +2749,26 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <v>1</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="14">
         <v>10.97</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="14">
         <f>G3*H3</f>
         <v>10.97</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <f>SUM(I3:I51)</f>
         <v>94.54000000000002</v>
       </c>
@@ -1160,23 +2783,23 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="11">
         <v>3</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="14">
         <v>0.92</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="14">
         <f t="shared" ref="I4:I67" si="0">G4*H4</f>
         <v>2.7600000000000002</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1190,23 +2813,23 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="11">
         <v>2</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="14">
         <v>1.17</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="14">
         <f t="shared" si="0"/>
         <v>2.34</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1220,23 +2843,23 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="11">
         <v>4</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="14">
         <v>0.23</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="14">
         <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1250,32 +2873,32 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="11">
         <v>6</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="14">
         <v>0.45</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="14">
         <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <f>SUM(I2:I100)</f>
         <v>94.54000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
@@ -1284,23 +2907,23 @@
       <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
         <v>38</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="11">
         <v>2</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="14">
         <v>2.04</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="14">
         <f t="shared" si="0"/>
         <v>4.08</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1314,23 +2937,23 @@
       <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
         <v>44</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="11">
         <v>4</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="13">
         <v>0.38</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="14">
         <f t="shared" si="0"/>
         <v>1.52</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1344,28 +2967,28 @@
       <c r="D10" t="s">
         <v>48</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="11">
         <v>2</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="13">
         <v>0.43</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="14">
         <f t="shared" si="0"/>
         <v>0.86</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C11" t="s">
@@ -1374,23 +2997,23 @@
       <c r="D11" t="s">
         <v>53</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
         <v>54</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="11">
         <v>1</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="13">
         <v>3.03</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="14">
         <f t="shared" si="0"/>
         <v>3.03</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1404,28 +3027,28 @@
       <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F12" t="s">
         <v>59</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="11">
         <v>60</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="13">
         <v>0.18</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="14">
         <f t="shared" si="0"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C13" t="s">
@@ -1434,28 +3057,28 @@
       <c r="D13" t="s">
         <v>65</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
         <v>66</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="11">
         <v>2</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="13">
         <v>0.73</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="14">
         <f t="shared" si="0"/>
         <v>1.46</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C14" t="s">
@@ -1464,28 +3087,28 @@
       <c r="D14" t="s">
         <v>70</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F14" t="s">
         <v>71</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="11">
         <v>2</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="13">
         <v>0.39</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="14">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="9" t="s">
         <v>63</v>
       </c>
       <c r="C15" t="s">
@@ -1494,23 +3117,23 @@
       <c r="D15" t="s">
         <v>73</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F15" t="s">
         <v>74</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="11">
         <v>1</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="13">
         <v>1.34</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="14">
         <f t="shared" si="0"/>
         <v>1.34</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1524,28 +3147,28 @@
       <c r="D16" t="s">
         <v>77</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
         <v>78</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="11">
         <v>1</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="13">
         <v>2.7</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="14">
         <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="7" t="s">
         <v>80</v>
       </c>
       <c r="C17" t="s">
@@ -1554,23 +3177,23 @@
       <c r="D17" t="s">
         <v>92</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F17" t="s">
         <v>93</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="11">
         <v>2</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="13">
         <v>3.26</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="14">
         <f t="shared" si="0"/>
         <v>6.52</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="4" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1584,23 +3207,23 @@
       <c r="D18" t="s">
         <v>89</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F18" t="s">
         <v>90</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="11">
         <v>1</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="13">
         <v>15.35</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="14">
         <f t="shared" si="0"/>
         <v>15.35</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1614,28 +3237,28 @@
       <c r="D19" t="s">
         <v>84</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F19" t="s">
         <v>85</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="11">
         <v>1</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="13">
         <v>5.29</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="14">
         <f t="shared" si="0"/>
         <v>5.29</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C20" t="s">
@@ -1644,28 +3267,28 @@
       <c r="D20">
         <v>1208</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F20" t="s">
         <v>97</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="11">
         <v>1</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="13">
         <v>4.95</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="14">
         <f t="shared" si="0"/>
         <v>4.95</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C21" t="s">
@@ -1674,28 +3297,28 @@
       <c r="D21" t="s">
         <v>101</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F21" t="s">
         <v>102</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="11">
         <v>1</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="13">
         <v>11.38</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="14">
         <f t="shared" si="0"/>
         <v>11.38</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C22" t="s">
@@ -1704,496 +3327,496 @@
       <c r="D22" t="s">
         <v>105</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F22" t="s">
         <v>106</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="11">
         <v>1</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="13">
         <v>4.79</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="14">
         <f t="shared" si="0"/>
         <v>4.79</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="4" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I23" s="2">
+      <c r="I23" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I24" s="2">
+      <c r="I24" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I25" s="2">
+      <c r="I25" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I26" s="2">
+      <c r="I26" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I27" s="2">
+      <c r="I27" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I28" s="2">
+      <c r="I28" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I29" s="2">
+      <c r="I29" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I30" s="2">
+      <c r="I30" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I31" s="2">
+      <c r="I31" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I32" s="2">
+      <c r="I32" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I33" s="2">
+      <c r="I33" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I34" s="2">
+      <c r="I34" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I35" s="2">
+      <c r="I35" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I36" s="2">
+      <c r="I36" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I37" s="2">
+      <c r="I37" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I38" s="2">
+      <c r="I38" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I39" s="2">
+      <c r="I39" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I40" s="2">
+      <c r="I40" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I41" s="2">
+      <c r="I41" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I42" s="2">
+      <c r="I42" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I43" s="2">
+      <c r="I43" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I44" s="2">
+      <c r="I44" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I45" s="2">
+      <c r="I45" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I46" s="2">
+      <c r="I46" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I47" s="2">
+      <c r="I47" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I48" s="2">
+      <c r="I48" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I49" s="2">
+      <c r="I49" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I50" s="2">
+      <c r="I50" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I51" s="2">
+      <c r="I51" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I52" s="2">
+      <c r="I52" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I53" s="2">
+      <c r="I53" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I54" s="2">
+      <c r="I54" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I55" s="2">
+      <c r="I55" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I56" s="2">
+      <c r="I56" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I57" s="2">
+      <c r="I57" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I58" s="2">
+      <c r="I58" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I59" s="2">
+      <c r="I59" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I60" s="2">
+      <c r="I60" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I61" s="2">
+      <c r="I61" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I62" s="2">
+      <c r="I62" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I63" s="2">
+      <c r="I63" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I64" s="2">
+      <c r="I64" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I65" s="2">
+      <c r="I65" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I66" s="2">
+      <c r="I66" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I67" s="2">
+      <c r="I67" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I68" s="2">
+      <c r="I68" s="14">
         <f t="shared" ref="I68:I101" si="1">G68*H68</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I69" s="2">
+      <c r="I69" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I70" s="2">
+      <c r="I70" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I71" s="2">
+      <c r="I71" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I72" s="2">
+      <c r="I72" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I73" s="2">
+      <c r="I73" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I74" s="2">
+      <c r="I74" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I75" s="2">
+      <c r="I75" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I76" s="2">
+      <c r="I76" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I77" s="2">
+      <c r="I77" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I78" s="2">
+      <c r="I78" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I79" s="2">
+      <c r="I79" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I80" s="2">
+      <c r="I80" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I81" s="2">
+      <c r="I81" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I82" s="2">
+      <c r="I82" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I83" s="2">
+      <c r="I83" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I84" s="2">
+      <c r="I84" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I85" s="2">
+      <c r="I85" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I86" s="2">
+      <c r="I86" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I87" s="2">
+      <c r="I87" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I88" s="2">
+      <c r="I88" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I89" s="2">
+      <c r="I89" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I90" s="2">
+      <c r="I90" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I91" s="2">
+      <c r="I91" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I92" s="2">
+      <c r="I92" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I93" s="2">
+      <c r="I93" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I94" s="2">
+      <c r="I94" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I95" s="2">
+      <c r="I95" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I96" s="2">
+      <c r="I96" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I97" s="2">
+      <c r="I97" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I98" s="2">
+      <c r="I98" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I99" s="2">
+      <c r="I99" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I100" s="2">
+      <c r="I100" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I101" s="2">
+      <c r="I101" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2229,13 +3852,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55AB20B3-088A-4C48-9746-FAFDBAF6F80B}">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2244,58 +3867,58 @@
     <col min="2" max="2" width="37.109375" customWidth="1"/>
     <col min="3" max="3" width="23.21875" customWidth="1"/>
     <col min="4" max="4" width="25.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="11" customWidth="1"/>
     <col min="6" max="6" width="35.109375" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="3"/>
-    <col min="9" max="9" width="17.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="13"/>
+    <col min="9" max="9" width="11.5546875" style="13" customWidth="1"/>
     <col min="10" max="10" width="35.5546875" customWidth="1"/>
     <col min="12" max="12" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="10" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2309,26 +3932,26 @@
       <c r="D3" t="s">
         <v>111</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
         <v>112</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <v>3</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="14">
         <v>0.24</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="14">
         <f t="shared" ref="I3:I69" si="0">G3*H3</f>
         <v>0.72</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <f>SUM(I3:I102)</f>
         <v>87.440000000000026</v>
       </c>
@@ -2343,23 +3966,23 @@
       <c r="D4" t="s">
         <v>115</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>116</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="11">
         <v>1</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="14">
         <v>2.69</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="14">
         <f t="shared" si="0"/>
         <v>2.69</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="3" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2373,23 +3996,23 @@
       <c r="D5" t="s">
         <v>120</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>121</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="11">
         <v>1</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="14">
         <v>11.56</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="14">
         <f t="shared" si="0"/>
         <v>11.56</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="3" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2403,23 +4026,23 @@
       <c r="D6">
         <v>1781</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>124</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="11">
         <v>1</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="14">
         <v>9.9499999999999993</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="14">
         <f t="shared" si="0"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="3" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2433,26 +4056,26 @@
       <c r="D7">
         <v>258</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
         <v>126</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="11">
         <v>1</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="14">
         <v>9.9499999999999993</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="14">
         <f t="shared" si="0"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -2464,23 +4087,23 @@
       <c r="D8">
         <v>1863</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
         <v>130</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="11">
         <v>1</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="14">
         <v>2.5</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="14">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="3" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2494,23 +4117,23 @@
       <c r="D9">
         <v>1304</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
         <v>132</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="11">
         <v>1</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="13">
         <v>5.95</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="14">
         <f t="shared" si="0"/>
         <v>5.95</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="3" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2524,23 +4147,23 @@
       <c r="D10" t="s">
         <v>136</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
         <v>137</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="11">
         <v>1</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="13">
         <v>3.03</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="14">
         <f t="shared" si="0"/>
         <v>3.03</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="3" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2554,23 +4177,23 @@
       <c r="D11" t="s">
         <v>140</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
         <v>141</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="11">
         <v>2</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="13">
         <v>0.75</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="14">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2584,23 +4207,23 @@
       <c r="D12" t="s">
         <v>150</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F12" t="s">
         <v>151</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="11">
         <v>1</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="13">
         <v>2.5299999999999998</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="14">
         <f t="shared" si="0"/>
         <v>2.5299999999999998</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="4" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2614,23 +4237,23 @@
       <c r="D13" t="s">
         <v>153</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
         <v>154</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="11">
         <v>1</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="13">
         <v>2.92</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="14">
         <f t="shared" si="0"/>
         <v>2.92</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2644,23 +4267,23 @@
       <c r="D14" t="s">
         <v>145</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F14" t="s">
         <v>146</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="11">
         <v>2</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="13">
         <v>1.65</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="14">
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="4" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2674,23 +4297,23 @@
       <c r="D15" t="s">
         <v>159</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F15" t="s">
         <v>160</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="11">
         <v>1</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="13">
         <v>4.82</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="14">
         <f t="shared" si="0"/>
         <v>4.82</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="4" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2704,23 +4327,23 @@
       <c r="D16" t="s">
         <v>181</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
         <v>182</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="11">
         <v>1</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="13">
         <v>1.05</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="14">
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="4" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2734,23 +4357,23 @@
       <c r="D17" t="s">
         <v>174</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F17" t="s">
         <v>175</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="11">
         <v>2</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="13">
         <v>6.61</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="14">
         <f t="shared" si="0"/>
         <v>13.22</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="4" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2764,23 +4387,23 @@
       <c r="D18" t="s">
         <v>178</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F18" t="s">
         <v>179</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="11">
         <v>1</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="13">
         <v>5.79</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="14">
         <f t="shared" si="0"/>
         <v>5.79</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="4" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2794,23 +4417,23 @@
       <c r="D19" t="s">
         <v>165</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F19" t="s">
         <v>167</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="11">
         <v>10</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="13">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="14">
         <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="4" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2824,23 +4447,23 @@
       <c r="D20" t="s">
         <v>170</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F20" t="s">
         <v>171</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="11">
         <v>10</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="13">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="14">
         <f t="shared" si="0"/>
         <v>0.44999999999999996</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="4" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2854,517 +4477,517 @@
       <c r="D21">
         <v>4149</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F21" t="s">
         <v>185</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="11">
         <v>1</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="13">
         <v>4.95</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="14">
         <f t="shared" si="0"/>
         <v>4.95</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="4" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="8"/>
+      <c r="I22" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="8"/>
+      <c r="I23" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="8"/>
+      <c r="I24" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I25" s="2">
+      <c r="I25" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I26" s="2">
+      <c r="I26" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I27" s="2">
+      <c r="I27" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I28" s="2">
+      <c r="I28" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I29" s="2">
+      <c r="I29" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I30" s="2">
+      <c r="I30" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I31" s="2">
+      <c r="I31" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I32" s="2">
+      <c r="I32" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I33" s="2">
+      <c r="I33" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I34" s="2">
+      <c r="I34" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I35" s="2">
+      <c r="I35" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I36" s="2">
+      <c r="I36" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I37" s="2">
+      <c r="I37" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I38" s="2">
+      <c r="I38" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I39" s="2">
+      <c r="I39" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I40" s="2">
+      <c r="I40" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I41" s="2">
+      <c r="I41" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I42" s="2">
+      <c r="I42" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I43" s="2">
+      <c r="I43" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I44" s="2">
+      <c r="I44" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I45" s="2">
+      <c r="I45" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I46" s="2">
+      <c r="I46" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I47" s="2">
+      <c r="I47" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I48" s="2">
+      <c r="I48" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I49" s="2">
+      <c r="I49" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I50" s="2">
+      <c r="I50" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I51" s="2">
+      <c r="I51" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I52" s="2">
+      <c r="I52" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I53" s="2">
+      <c r="I53" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I54" s="2">
+      <c r="I54" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I55" s="2">
+      <c r="I55" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I56" s="2">
+      <c r="I56" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I57" s="2">
+      <c r="I57" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I58" s="2">
+      <c r="I58" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I59" s="2">
+      <c r="I59" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I60" s="2">
+      <c r="I60" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I61" s="2">
+      <c r="I61" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I62" s="2">
+      <c r="I62" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I63" s="2">
+      <c r="I63" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I64" s="2">
+      <c r="I64" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I65" s="2">
+      <c r="I65" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I66" s="2">
+      <c r="I66" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I67" s="2">
+      <c r="I67" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I68" s="2">
+      <c r="I68" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I69" s="2">
+      <c r="I69" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I70" s="2">
+      <c r="I70" s="14">
         <f t="shared" ref="I70:I103" si="1">G70*H70</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I71" s="2">
+      <c r="I71" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I72" s="2">
+      <c r="I72" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I73" s="2">
+      <c r="I73" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I74" s="2">
+      <c r="I74" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I75" s="2">
+      <c r="I75" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I76" s="2">
+      <c r="I76" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I77" s="2">
+      <c r="I77" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I78" s="2">
+      <c r="I78" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I79" s="2">
+      <c r="I79" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I80" s="2">
+      <c r="I80" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I81" s="2">
+      <c r="I81" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I82" s="2">
+      <c r="I82" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I83" s="2">
+      <c r="I83" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I84" s="2">
+      <c r="I84" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I85" s="2">
+      <c r="I85" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I86" s="2">
+      <c r="I86" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I87" s="2">
+      <c r="I87" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I88" s="2">
+      <c r="I88" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I89" s="2">
+      <c r="I89" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I90" s="2">
+      <c r="I90" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I91" s="2">
+      <c r="I91" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I92" s="2">
+      <c r="I92" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I93" s="2">
+      <c r="I93" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I94" s="2">
+      <c r="I94" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I95" s="2">
+      <c r="I95" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I96" s="2">
+      <c r="I96" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I97" s="2">
+      <c r="I97" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I98" s="2">
+      <c r="I98" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I99" s="2">
+      <c r="I99" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I100" s="2">
+      <c r="I100" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I101" s="2">
+      <c r="I101" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I102" s="2">
+      <c r="I102" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I103" s="2">
+      <c r="I103" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Potentially solved LED driving problem. We'll see.
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4AA60C-1018-47A9-A462-8E0CDDE39BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7760EA09-5526-48B6-9A99-B5AAD997D1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="201">
   <si>
     <t>Quantity</t>
   </si>
@@ -637,6 +637,9 @@
   </si>
   <si>
     <t xml:space="preserve">battery management IC stuff </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debouncing ICs? </t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1110,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,6 +1283,9 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>200</v>
+      </c>
       <c r="I11" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1644,7 +1650,7 @@
     </row>
     <row r="69" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I69" s="14">
-        <f t="shared" ref="I69:I132" si="1">G69*H69</f>
+        <f t="shared" ref="I69:I104" si="1">G69*H69</f>
         <v>0</v>
       </c>
     </row>
@@ -2051,7 +2057,7 @@
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14">
-        <f t="shared" ref="I7:I70" si="1">G8*H8</f>
+        <f t="shared" ref="I8:I70" si="1">G8*H8</f>
         <v>0</v>
       </c>
       <c r="J8" s="3"/>

</xml_diff>

<commit_message>
Add some PCB work. Lots of unfinished nets.
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7760EA09-5526-48B6-9A99-B5AAD997D1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B052B2-ABA4-4CBF-AA6B-8157E80BC7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="205">
   <si>
     <t>Quantity</t>
   </si>
@@ -640,6 +640,18 @@
   </si>
   <si>
     <t xml:space="preserve">Debouncing ICs? </t>
+  </si>
+  <si>
+    <t>POGO Pins</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/3m/D2510-6V0C-AR-WD/1886332</t>
+  </si>
+  <si>
+    <t>D2510-6V0C-AR-WD</t>
+  </si>
+  <si>
+    <t>MSH10ECT-ND</t>
   </si>
 </sst>
 </file>
@@ -1108,9 +1120,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535EBE7C-EB1B-4F48-8827-B2C8DF8DD54E}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1293,6 +1305,9 @@
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>201</v>
+      </c>
       <c r="I12" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1877,9 +1892,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F9AC-3655-4B8A-AD78-25E473D1BEC8}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1951,7 +1966,7 @@
       <c r="J3" s="4"/>
       <c r="L3" s="2">
         <f>SUM(I3:I105)</f>
-        <v>12.370000000000001</v>
+        <v>14.41</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2029,26 +2044,26 @@
         <v>135</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>203</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>141</v>
+        <v>204</v>
       </c>
       <c r="G7" s="11">
         <v>1</v>
       </c>
       <c r="H7" s="13">
-        <v>0.75</v>
+        <v>2.79</v>
       </c>
       <c r="I7" s="14">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>2.79</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>142</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2669,9 +2684,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J5" r:id="rId1" xr:uid="{6CAFF770-2D29-4F0D-A99E-4F828E77668E}"/>
+    <hyperlink ref="J7" r:id="rId2" xr:uid="{F3DC198F-993B-48F6-8A2B-9352196B79BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Finish digit 0 schematic (colored yellow.)
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B052B2-ABA4-4CBF-AA6B-8157E80BC7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC16F366-5D96-455D-A32A-1C24680764AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="216">
   <si>
     <t>Quantity</t>
   </si>
@@ -652,6 +652,39 @@
   </si>
   <si>
     <t>MSH10ECT-ND</t>
+  </si>
+  <si>
+    <t>150060RS75000</t>
+  </si>
+  <si>
+    <t>732-4978-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green SMT LEDs (surface mount) </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/150060RS75000/4489901</t>
+  </si>
+  <si>
+    <t>155124RS73200</t>
+  </si>
+  <si>
+    <t>732-5025-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/155124RS73200/4490041</t>
+  </si>
+  <si>
+    <t>Lite-On Inc.</t>
+  </si>
+  <si>
+    <t>LTST-C191KGKT</t>
+  </si>
+  <si>
+    <t>160-1446-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/liteon/LTST-C191KGKT/386835</t>
   </si>
 </sst>
 </file>
@@ -1890,11 +1923,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F9AC-3655-4B8A-AD78-25E473D1BEC8}">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1962,719 +1995,789 @@
       <c r="B3" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="4"/>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="11">
+        <v>56</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="I3" s="14">
+        <f t="shared" ref="I3:I6" si="0">G3*H3</f>
+        <v>7.9519999999999991</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>208</v>
+      </c>
       <c r="L3" s="2">
-        <f>SUM(I3:I105)</f>
-        <v>14.41</v>
+        <f>SUM(I3:I106)</f>
+        <v>22.761999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>188</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="4"/>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G4" s="11">
+        <v>2</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="I4" s="14">
+        <f t="shared" ref="I4:I8" si="1">G4*H4</f>
+        <v>0.4</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>212</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>213</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G5" s="11">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13">
-        <v>11.38</v>
+        <v>214</v>
       </c>
       <c r="I5" s="14">
-        <f t="shared" ref="I5:I7" si="0">G5*H5</f>
-        <v>11.38</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>103</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G6" s="11">
         <v>1</v>
       </c>
-      <c r="H6" s="14">
-        <v>0.24</v>
+      <c r="H6" s="13">
+        <v>11.38</v>
       </c>
       <c r="I6" s="14">
         <f t="shared" si="0"/>
-        <v>0.24</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>108</v>
+        <v>11.38</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>194</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
+        <v>111</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>204</v>
+        <v>112</v>
       </c>
       <c r="G7" s="11">
         <v>1</v>
       </c>
-      <c r="H7" s="13">
-        <v>2.79</v>
+      <c r="H7" s="14">
+        <v>0.24</v>
       </c>
       <c r="I7" s="14">
-        <f t="shared" si="0"/>
-        <v>2.79</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>202</v>
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>189</v>
-      </c>
-      <c r="H8" s="14"/>
+        <v>194</v>
+      </c>
+      <c r="C8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>2.79</v>
+      </c>
       <c r="I8" s="14">
-        <f t="shared" ref="I8:I70" si="1">G8*H8</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="L8" s="2"/>
+        <f t="shared" si="1"/>
+        <v>2.79</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I9:I71" si="2">G9*H9</f>
         <v>0</v>
       </c>
       <c r="J9" s="3"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>190</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>191</v>
       </c>
-      <c r="I10" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I11" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I12" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="4"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I13" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I14" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I15" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I16" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I17" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I18" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I19" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I20" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I21" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I22" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I23" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I24" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I25" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I26" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I27" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I28" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I29" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I30" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I31" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I32" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I33" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I34" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I35" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I36" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I37" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I38" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I39" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I40" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I41" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I42" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I43" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I44" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I45" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I46" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I47" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I48" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I49" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I50" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I51" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I52" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I53" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I54" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I55" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I56" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I57" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I58" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I59" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I60" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I61" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I62" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I63" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I64" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I65" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I66" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I67" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I68" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I69" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I70" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I71" s="14">
-        <f t="shared" ref="I71:I104" si="2">G71*H71</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I72" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I72:I105" si="3">G72*H72</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I73" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I74" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I75" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I76" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I77" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I78" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I79" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I80" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I81" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I82" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I83" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I84" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I85" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I86" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I87" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I88" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I89" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I90" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I91" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I92" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I93" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I94" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I95" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I96" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I97" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I98" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I99" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I100" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I101" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I102" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I103" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I104" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I105" s="14">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2683,8 +2786,8 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J5" r:id="rId1" xr:uid="{6CAFF770-2D29-4F0D-A99E-4F828E77668E}"/>
-    <hyperlink ref="J7" r:id="rId2" xr:uid="{F3DC198F-993B-48F6-8A2B-9352196B79BD}"/>
+    <hyperlink ref="J6" r:id="rId1" xr:uid="{6CAFF770-2D29-4F0D-A99E-4F828E77668E}"/>
+    <hyperlink ref="J8" r:id="rId2" xr:uid="{F3DC198F-993B-48F6-8A2B-9352196B79BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Add to main schematic - need segemtn driver and off-board connections/ports. Also - verify that I do not need to talk to cap. touch through I2C.
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC16F366-5D96-455D-A32A-1C24680764AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AA4BF0-2E89-4AB1-A0D0-ACD72F339610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="222">
   <si>
     <t>Quantity</t>
   </si>
@@ -685,6 +685,24 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/liteon/LTST-C191KGKT/386835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear 5V Regulator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear 3.3V Regulator </t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>AZ1117IH-3.3TRG1</t>
+  </si>
+  <si>
+    <t>AZ1117IH-3.3TRG1DICT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
   </si>
 </sst>
 </file>
@@ -1923,11 +1941,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F9AC-3655-4B8A-AD78-25E473D1BEC8}">
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17:D18"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2021,8 +2039,8 @@
         <v>208</v>
       </c>
       <c r="L3" s="2">
-        <f>SUM(I3:I106)</f>
-        <v>22.761999999999997</v>
+        <f>SUM(I3:I108)</f>
+        <v>23.131999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2048,7 +2066,7 @@
         <v>0.2</v>
       </c>
       <c r="I4" s="14">
-        <f t="shared" ref="I4:I8" si="1">G4*H4</f>
+        <f t="shared" ref="I4:I10" si="1">G4*H4</f>
         <v>0.4</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -2170,58 +2188,84 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>189</v>
-      </c>
-      <c r="H9" s="14"/>
+      <c r="B9" s="8" t="s">
+        <v>216</v>
+      </c>
       <c r="I9" s="14">
-        <f t="shared" ref="I9:I71" si="2">G9*H9</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="L9" s="2"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>190</v>
-      </c>
-      <c r="H10" s="14"/>
+        <v>217</v>
+      </c>
+      <c r="C10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" t="s">
+        <v>219</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>220</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0.37</v>
+      </c>
       <c r="I10" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="3"/>
+        <f t="shared" si="1"/>
+        <v>0.37</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>189</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14">
+        <f t="shared" ref="I11:I73" si="2">G11*H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>191</v>
       </c>
-      <c r="I11" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I12" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="4"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I14" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="4"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I15" s="14">
@@ -2312,12 +2356,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="J27" s="4"/>
     </row>
     <row r="28" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I28" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="J28" s="4"/>
     </row>
     <row r="29" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I29" s="14">
@@ -2579,19 +2625,19 @@
     </row>
     <row r="72" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I72" s="14">
-        <f t="shared" ref="I72:I105" si="3">G72*H72</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I73" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I74" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I74:I107" si="3">G74*H74</f>
         <v>0</v>
       </c>
     </row>
@@ -2777,6 +2823,18 @@
     </row>
     <row r="105" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I105" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I106" s="14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I107" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2788,9 +2846,10 @@
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1" xr:uid="{6CAFF770-2D29-4F0D-A99E-4F828E77668E}"/>
     <hyperlink ref="J8" r:id="rId2" xr:uid="{F3DC198F-993B-48F6-8A2B-9352196B79BD}"/>
+    <hyperlink ref="J3" r:id="rId3" xr:uid="{7FF614E6-9214-4B15-B18D-F37EF6411D92}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Big parameter mods to BOM and to libraries. Forcing overwrite of STM32.
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AA4BF0-2E89-4AB1-A0D0-ACD72F339610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8D3621-B5D1-43E8-A4D0-17FD00FEC407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="259">
   <si>
     <t>Quantity</t>
   </si>
@@ -600,21 +600,6 @@
     <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/4149/10123800</t>
   </si>
   <si>
-    <t>Red SMT LEDs (surface mount)</t>
-  </si>
-  <si>
-    <t>Red SMT LEDs (surface mount, right angle)</t>
-  </si>
-  <si>
-    <t>MOSFETS</t>
-  </si>
-  <si>
-    <t>caps.</t>
-  </si>
-  <si>
-    <t>res.</t>
-  </si>
-  <si>
     <t>STM32</t>
   </si>
   <si>
@@ -645,24 +630,12 @@
     <t>POGO Pins</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/3m/D2510-6V0C-AR-WD/1886332</t>
-  </si>
-  <si>
-    <t>D2510-6V0C-AR-WD</t>
-  </si>
-  <si>
-    <t>MSH10ECT-ND</t>
-  </si>
-  <si>
     <t>150060RS75000</t>
   </si>
   <si>
     <t>732-4978-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Green SMT LEDs (surface mount) </t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/150060RS75000/4489901</t>
   </si>
   <si>
@@ -675,24 +648,6 @@
     <t>https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/155124RS73200/4490041</t>
   </si>
   <si>
-    <t>Lite-On Inc.</t>
-  </si>
-  <si>
-    <t>LTST-C191KGKT</t>
-  </si>
-  <si>
-    <t>160-1446-1-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/liteon/LTST-C191KGKT/386835</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linear 5V Regulator </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linear 3.3V Regulator </t>
-  </si>
-  <si>
     <t>Diodes Incorporated</t>
   </si>
   <si>
@@ -703,6 +658,162 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>5988070107F</t>
+  </si>
+  <si>
+    <t>Dialight</t>
+  </si>
+  <si>
+    <t>350-2035-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/dialight/5988070107F/1291269</t>
+  </si>
+  <si>
+    <t>Capacitor - 10uF, 0402</t>
+  </si>
+  <si>
+    <t>Resistor - 56 ohm, 0402</t>
+  </si>
+  <si>
+    <t>Resistor - 240 ohm, 0402</t>
+  </si>
+  <si>
+    <t>Resistor - 10k ohm, 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-channel MOSFET - SOT-23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Point - Surface Mount </t>
+  </si>
+  <si>
+    <t>Linear 3.3V Regulator - SOT-223-3</t>
+  </si>
+  <si>
+    <t>8-bit shift Shift Register - 16-TSSOP</t>
+  </si>
+  <si>
+    <t>74HC595PW,118</t>
+  </si>
+  <si>
+    <t>Nexperia USA Inc.</t>
+  </si>
+  <si>
+    <t>1727-3068-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nexperia-usa-inc/74HC595PW-118/946653</t>
+  </si>
+  <si>
+    <t>Resistor Network - 8-pos, 8.2K</t>
+  </si>
+  <si>
+    <t>Red SMT LED - surface mount, 0603</t>
+  </si>
+  <si>
+    <t>Red SMT LEDs - surface mount, right angle, 1206</t>
+  </si>
+  <si>
+    <t>Green SMT LEDs - surface mount, 0603</t>
+  </si>
+  <si>
+    <t>MNR18ERAPJ822</t>
+  </si>
+  <si>
+    <t>Rohm Semiconductor</t>
+  </si>
+  <si>
+    <t>511-MNR18ERAPJ822CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/MNR18ERAPJ822/4083449</t>
+  </si>
+  <si>
+    <t>DMN63D8L-7</t>
+  </si>
+  <si>
+    <t>DMN63D8L-7DICT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/DMN63D8L-7/5699705</t>
+  </si>
+  <si>
+    <t>GRM155R61A106ME11D</t>
+  </si>
+  <si>
+    <t>490-GRM155R61A106ME11DCT-ND</t>
+  </si>
+  <si>
+    <t>Capacitor - 1uF, 0402</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/GRM155R61A106ME11D/12091056</t>
+  </si>
+  <si>
+    <t>CL05A105KP5NNNC</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>1276-1076-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05A105KP5NNNC/3886734</t>
+  </si>
+  <si>
+    <t>RC0402FR-0756RL</t>
+  </si>
+  <si>
+    <t>311-56.0LRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0402FR-0756RL/726636</t>
+  </si>
+  <si>
+    <t>Resistor - 330 ohm, 0402</t>
+  </si>
+  <si>
+    <t>RC0402JR-13330RL</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0402JR-13330RL/14008183</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0402FR-07240RL/2827564</t>
+  </si>
+  <si>
+    <t>RC0402FR-07240RL</t>
+  </si>
+  <si>
+    <t>311-240LRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402JR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10KJRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0402JR-0710KL/726418</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RCWCTE/11476558</t>
+  </si>
+  <si>
+    <t>KOA Speer Electronics, Inc.</t>
+  </si>
+  <si>
+    <t>RCWCTE</t>
+  </si>
+  <si>
+    <t>2019-RCWCTECT-ND</t>
   </si>
 </sst>
 </file>
@@ -846,7 +957,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -881,6 +992,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1173,7 +1293,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1239,7 +1359,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I3" s="14">
         <f t="shared" ref="I3:I68" si="0">G3*H3</f>
@@ -1248,12 +1368,12 @@
       <c r="J3" s="4"/>
       <c r="L3" s="2">
         <f>SUM(I3:I105)</f>
-        <v>0.75</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I4" s="14">
         <f t="shared" si="0"/>
@@ -1263,7 +1383,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
         <v>135</v>
@@ -1293,7 +1413,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14">
@@ -1304,7 +1424,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I7" s="14">
         <f t="shared" si="0"/>
@@ -1314,7 +1434,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14">
@@ -1326,7 +1446,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14">
@@ -1337,7 +1457,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I10" s="14">
         <f t="shared" si="0"/>
@@ -1347,7 +1467,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I11" s="14">
         <f t="shared" si="0"/>
@@ -1357,7 +1477,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I12" s="14">
         <f t="shared" si="0"/>
@@ -1366,11 +1486,34 @@
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" s="14">
+        <v>0.24</v>
+      </c>
       <c r="I13" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="4"/>
+        <f>G13*H13</f>
+        <v>0.24</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I14" s="14">
@@ -1941,17 +2084,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F9AC-3655-4B8A-AD78-25E473D1BEC8}">
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.21875" customWidth="1"/>
     <col min="4" max="4" width="25.88671875" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" style="11" customWidth="1"/>
@@ -2011,19 +2154,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>187</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G3" s="11">
         <v>56</v>
@@ -2032,32 +2175,32 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="I3" s="14">
-        <f t="shared" ref="I3:I6" si="0">G3*H3</f>
+        <f>G3*H3</f>
         <v>7.9519999999999991</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="L3" s="2">
-        <f>SUM(I3:I108)</f>
-        <v>23.131999999999998</v>
+        <f>SUM(I3:I111)</f>
+        <v>20.738</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>188</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G4" s="11">
         <v>2</v>
@@ -2066,776 +2209,957 @@
         <v>0.2</v>
       </c>
       <c r="I4" s="14">
-        <f t="shared" ref="I4:I10" si="1">G4*H4</f>
+        <f>G4*H4</f>
         <v>0.4</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" t="s">
         <v>207</v>
       </c>
-      <c r="C5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" t="s">
-        <v>213</v>
-      </c>
       <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>214</v>
+        <v>209</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.32</v>
       </c>
       <c r="I5" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>G5*H5</f>
+        <v>0.32</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>99</v>
+        <v>218</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>219</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>221</v>
       </c>
       <c r="G6" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H6" s="13">
-        <v>11.38</v>
+        <v>0.47</v>
       </c>
       <c r="I6" s="14">
-        <f t="shared" si="0"/>
-        <v>11.38</v>
+        <f t="shared" ref="I6:I17" si="0">G6*H6</f>
+        <v>1.88</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>103</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>109</v>
+        <v>223</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>228</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>227</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>112</v>
+        <v>229</v>
       </c>
       <c r="G7" s="11">
+        <v>4</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="11">
         <v>1</v>
       </c>
-      <c r="H7" s="14">
-        <v>0.24</v>
-      </c>
-      <c r="I7" s="14">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" t="s">
-        <v>203</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>204</v>
-      </c>
-      <c r="G8" s="11">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13">
-        <v>2.79</v>
-      </c>
-      <c r="I8" s="14">
-        <f t="shared" si="1"/>
-        <v>2.79</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>216</v>
+      <c r="H9" s="13">
+        <v>0.37</v>
       </c>
       <c r="I9" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="4"/>
+        <f t="shared" si="0"/>
+        <v>0.37</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D10" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="G10" s="11">
-        <v>1</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0.37</v>
+        <v>23</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0.192</v>
       </c>
       <c r="I10" s="14">
-        <f t="shared" si="1"/>
-        <v>0.37</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>221</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>4.4160000000000004</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>189</v>
-      </c>
-      <c r="H11" s="14"/>
+        <v>211</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>235</v>
+      </c>
+      <c r="G11" s="11">
+        <v>3</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0.12</v>
+      </c>
       <c r="I11" s="14">
-        <f t="shared" ref="I11:I73" si="2">G11*H11</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="3"/>
-      <c r="L11" s="2"/>
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>190</v>
-      </c>
-      <c r="H12" s="14"/>
+        <v>236</v>
+      </c>
+      <c r="C12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" t="s">
+        <v>238</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>240</v>
+      </c>
+      <c r="G12" s="11">
+        <v>4</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.1</v>
+      </c>
       <c r="I12" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>191</v>
+        <v>212</v>
+      </c>
+      <c r="C13" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>243</v>
+      </c>
+      <c r="G13" s="11">
+        <v>3</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0.1</v>
       </c>
       <c r="I13" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="G14" s="20">
+        <v>11</v>
+      </c>
+      <c r="H14" s="21">
+        <v>0.1</v>
+      </c>
       <c r="I14" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="3"/>
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>251</v>
+      </c>
+      <c r="G15" s="11">
+        <v>12</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0.1</v>
+      </c>
       <c r="I15" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="4"/>
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" t="s">
+        <v>252</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>253</v>
+      </c>
+      <c r="G16" s="11">
+        <v>2</v>
+      </c>
+      <c r="H16" s="13">
+        <v>0.1</v>
+      </c>
       <c r="I16" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" t="s">
+        <v>256</v>
+      </c>
+      <c r="D17" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>258</v>
+      </c>
+      <c r="G17" s="11">
+        <v>9</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0.16</v>
+      </c>
       <c r="I17" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1.44</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I18" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I18:I76" si="1">G18*H18</f>
         <v>0</v>
       </c>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I19" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I21" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I22" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I23" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I24" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I25" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I26" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I27" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I28" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I29" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="9:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I30" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="9:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I31" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="9:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I32" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I33" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I34" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I35" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I36" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I37" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I38" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I39" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I40" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I41" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I42" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I43" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I44" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I45" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I46" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I47" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I48" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I49" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I50" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I51" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I52" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I53" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I54" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I55" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I56" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I57" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I58" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I59" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I60" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I61" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I62" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I63" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I64" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I65" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I66" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I67" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I68" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I69" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I70" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I71" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I72" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I73" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I74" s="14">
-        <f t="shared" ref="I74:I107" si="3">G74*H74</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I75" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I76" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I77" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I77:I110" si="2">G77*H77</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I78" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I79" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I80" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I81" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I82" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I83" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I84" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I85" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I86" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I87" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I88" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I89" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I90" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I91" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I92" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I93" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I94" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I95" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I96" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I97" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I98" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I99" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I100" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I101" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I102" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I103" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I104" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I105" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I106" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I107" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I108" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I109" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I110" s="14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2844,9 +3168,9 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J6" r:id="rId1" xr:uid="{6CAFF770-2D29-4F0D-A99E-4F828E77668E}"/>
-    <hyperlink ref="J8" r:id="rId2" xr:uid="{F3DC198F-993B-48F6-8A2B-9352196B79BD}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{7FF614E6-9214-4B15-B18D-F37EF6411D92}"/>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{7FF614E6-9214-4B15-B18D-F37EF6411D92}"/>
+    <hyperlink ref="J7" r:id="rId2" xr:uid="{06FBC2E7-7499-4DE3-82D0-4097CE0647AA}"/>
+    <hyperlink ref="J13" r:id="rId3" xr:uid="{E998AA30-CA0E-4463-A55C-ED48248E9895}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
BOM changes are complete. Test points need to be finally placed/routed, and schem. parameters updated.
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8D3621-B5D1-43E8-A4D0-17FD00FEC407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8E2A18-3BC5-47C8-BC86-03A2B40B0BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2088,7 +2088,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
PN parameters added to components. Resistor values adjusted.
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mhofmeister\Documents\clk\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8E2A18-3BC5-47C8-BC86-03A2B40B0BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B865BEE-3545-409F-8EBB-601B7AEFE2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="259">
   <si>
     <t>Quantity</t>
   </si>
@@ -914,7 +914,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -948,6 +948,32 @@
       <top/>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -992,15 +1018,21 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2088,7 +2120,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2106,49 +2138,47 @@
     <col min="12" max="12" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-    </row>
-    <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15"/>
-      <c r="B2" s="10" t="s">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:12" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="21" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2183,7 +2213,7 @@
       </c>
       <c r="L3" s="2">
         <f>SUM(I3:I111)</f>
-        <v>20.738</v>
+        <v>20.937999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2457,55 +2487,54 @@
         <v>243</v>
       </c>
       <c r="G13" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H13" s="13">
         <v>0.1</v>
       </c>
       <c r="I13" s="14">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>245</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" t="s">
         <v>247</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" t="s">
         <v>246</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" t="s">
         <v>246</v>
       </c>
-      <c r="G14" s="20">
-        <v>11</v>
-      </c>
-      <c r="H14" s="21">
+      <c r="G14" s="11">
+        <v>12</v>
+      </c>
+      <c r="H14" s="13">
         <v>0.1</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J14" s="22" t="s">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+      <c r="B15" t="s">
         <v>213</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" t="s">
         <v>247</v>
       </c>
       <c r="D15" t="s">
@@ -2518,24 +2547,24 @@
         <v>251</v>
       </c>
       <c r="G15" s="11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15" s="13">
         <v>0.1</v>
       </c>
       <c r="I15" s="14">
         <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
+      <c r="B16" t="s">
         <v>214</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" t="s">
         <v>247</v>
       </c>
       <c r="D16" t="s">

</xml_diff>

<commit_message>
Add ZAMM graphic. Add PCB connector to BOM.
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mhofmeister\Documents\clk\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B865BEE-3545-409F-8EBB-601B7AEFE2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2B36FC-B4A3-4843-9E20-DFA02578BE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="264">
   <si>
     <t>Quantity</t>
   </si>
@@ -814,6 +814,21 @@
   </si>
   <si>
     <t>2019-RCWCTECT-ND</t>
+  </si>
+  <si>
+    <t>Connector - Male Receptacle, 5x2 pos, 0.1" pitch</t>
+  </si>
+  <si>
+    <t>CNC Tech</t>
+  </si>
+  <si>
+    <t>3020-10-0300-00</t>
+  </si>
+  <si>
+    <t>1175-1621-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cnc-tech/3020-10-0300-00/3441727</t>
   </si>
 </sst>
 </file>
@@ -983,7 +998,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1012,18 +1027,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1033,6 +1036,19 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1344,17 +1360,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
@@ -2118,17 +2134,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F9AC-3655-4B8A-AD78-25E473D1BEC8}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" style="11" customWidth="1"/>
     <col min="5" max="5" width="16.77734375" style="11" customWidth="1"/>
     <col min="6" max="6" width="35.109375" customWidth="1"/>
     <col min="7" max="7" width="9" style="11" customWidth="1"/>
@@ -2139,46 +2155,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-    </row>
-    <row r="2" spans="1:12" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21" t="s">
+      <c r="A1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+    </row>
+    <row r="2" spans="1:12" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="22" t="s">
+      <c r="G2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="17" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2186,10 +2202,10 @@
       <c r="B3" t="s">
         <v>224</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
         <v>197</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -2213,17 +2229,17 @@
       </c>
       <c r="L3" s="2">
         <f>SUM(I3:I111)</f>
-        <v>20.937999999999999</v>
+        <v>21.617999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>225</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="11" t="s">
         <v>200</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -2250,10 +2266,10 @@
       <c r="B5" t="s">
         <v>226</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="11" t="s">
         <v>207</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -2280,10 +2296,10 @@
       <c r="B6" t="s">
         <v>218</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="11" t="s">
         <v>219</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -2310,10 +2326,10 @@
       <c r="B7" t="s">
         <v>223</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="11" t="s">
         <v>227</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -2337,26 +2353,43 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
-        <v>189</v>
+      <c r="B8" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>261</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="F8" t="s">
+        <v>262</v>
+      </c>
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0.68</v>
+      </c>
       <c r="I8" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="4"/>
+        <v>0.68</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>217</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="11" t="s">
         <v>204</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -2383,10 +2416,10 @@
       <c r="B10" t="s">
         <v>215</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="11" t="s">
         <v>231</v>
       </c>
       <c r="E10" s="11" t="s">
@@ -2414,10 +2447,10 @@
       <c r="B11" t="s">
         <v>211</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="11" t="s">
         <v>234</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -2444,10 +2477,10 @@
       <c r="B12" t="s">
         <v>236</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="11" t="s">
         <v>238</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -2474,10 +2507,10 @@
       <c r="B13" t="s">
         <v>212</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="11" t="s">
         <v>242</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -2504,10 +2537,10 @@
       <c r="B14" t="s">
         <v>245</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="11" t="s">
         <v>246</v>
       </c>
       <c r="E14" s="11" t="s">
@@ -2534,10 +2567,10 @@
       <c r="B15" t="s">
         <v>213</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="11" t="s">
         <v>250</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -2564,10 +2597,10 @@
       <c r="B16" t="s">
         <v>214</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="11" t="s">
         <v>252</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -2594,10 +2627,10 @@
       <c r="B17" t="s">
         <v>216</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="11" t="s">
         <v>257</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -3231,17 +3264,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
@@ -4414,17 +4447,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>

</xml_diff>

<commit_message>
PR-3 has been purchased
</commit_message>
<xml_diff>
--- a/sinking-clock-BOM-v2.xlsx
+++ b/sinking-clock-BOM-v2.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mhofmeister\Documents\clk\sinking-clock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2B36FC-B4A3-4843-9E20-DFA02578BE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E4A317-98D1-4431-A974-B1A2758613D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
     <sheet name="LED PCB Assembly" sheetId="5" r:id="rId2"/>
     <sheet name="PR-1" sheetId="1" r:id="rId3"/>
     <sheet name="PR-2" sheetId="3" r:id="rId4"/>
+    <sheet name="PR-3" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="295">
   <si>
     <t>Quantity</t>
   </si>
@@ -829,6 +830,99 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/cnc-tech/3020-10-0300-00/3441727</t>
+  </si>
+  <si>
+    <t>LED PCB Components</t>
+  </si>
+  <si>
+    <t>STM32 ST-Link V2 In-circuit Debugger</t>
+  </si>
+  <si>
+    <t>ST-LINK/V2</t>
+  </si>
+  <si>
+    <t>497-10484-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/ST-LINK-V2/2214535</t>
+  </si>
+  <si>
+    <t>Plug-of-Nails POGO-pin SWD connector</t>
+  </si>
+  <si>
+    <t>Tag-Connect LLC</t>
+  </si>
+  <si>
+    <t>TC2030-IDC</t>
+  </si>
+  <si>
+    <t>TC2030-IDC-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tag-connect-llc/TC2030-IDC/4571121</t>
+  </si>
+  <si>
+    <t>ChipQuik Solder Paste</t>
+  </si>
+  <si>
+    <t>SMD291AX10</t>
+  </si>
+  <si>
+    <t>SMD291AX10-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/chip-quik-inc/SMD291AX10/2057271</t>
+  </si>
+  <si>
+    <t>E-Switch</t>
+  </si>
+  <si>
+    <t>TL3305AF260QG</t>
+  </si>
+  <si>
+    <t>EG5353CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/e-switch/TL3305AF260QG/5816184</t>
+  </si>
+  <si>
+    <t>Tactile push button Switch - option 1: 3.8mm</t>
+  </si>
+  <si>
+    <t>Tactile push button Switch - option 2: 8.5mm</t>
+  </si>
+  <si>
+    <t>TL3301PF160QG</t>
+  </si>
+  <si>
+    <t>EG4562CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/e-switch/TL3301PF160QG/1756542</t>
+  </si>
+  <si>
+    <t>Tactile push button Switch - option 3: 9.5mm</t>
+  </si>
+  <si>
+    <t>TL3301BF160QGTUBE</t>
+  </si>
+  <si>
+    <t>141-TL3301BF160QGTUBE-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/e-switch/TL3301BF160QGTUBE/1805543</t>
+  </si>
+  <si>
+    <t>Tactile push button Switch - option 4: 13.0mm</t>
+  </si>
+  <si>
+    <t>TL3301DF160QG</t>
+  </si>
+  <si>
+    <t>EG5463CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/e-switch/TL3301DF160QG/1805555</t>
   </si>
 </sst>
 </file>
@@ -839,7 +933,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -884,8 +978,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -925,6 +1025,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,7 +1104,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1048,7 +1154,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2134,9 +2265,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF30F9AC-3655-4B8A-AD78-25E473D1BEC8}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2353,7 +2484,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
+      <c r="B8" t="s">
         <v>259</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -5573,4 +5704,1386 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B494BF-8FB3-4F10-BF9B-C1AB6CBBBD39}">
+  <dimension ref="A1:L102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="35.109375" customWidth="1"/>
+    <col min="7" max="7" width="9" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="13"/>
+    <col min="9" max="9" width="11.5546875" style="13" customWidth="1"/>
+    <col min="10" max="10" width="35.5546875" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" s="24">
+        <v>168</v>
+      </c>
+      <c r="H3" s="25">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="I3" s="26">
+        <f>G3*H3</f>
+        <v>23.855999999999998</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="L3" s="2">
+        <f>SUM(I3:I101)</f>
+        <v>153.68399999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" s="24">
+        <v>6</v>
+      </c>
+      <c r="H4" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="I4" s="26">
+        <f>G4*H4</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="G5" s="24">
+        <v>3</v>
+      </c>
+      <c r="H5" s="25">
+        <v>0.32</v>
+      </c>
+      <c r="I5" s="26">
+        <f>G5*H5</f>
+        <v>0.96</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="G6" s="24">
+        <v>12</v>
+      </c>
+      <c r="H6" s="25">
+        <v>0.47</v>
+      </c>
+      <c r="I6" s="26">
+        <f t="shared" ref="I6:I17" si="0">G6*H6</f>
+        <v>5.64</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="G7" s="24">
+        <v>12</v>
+      </c>
+      <c r="H7" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="26">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="G8" s="24">
+        <v>3</v>
+      </c>
+      <c r="H8" s="25">
+        <v>0.68</v>
+      </c>
+      <c r="I8" s="26">
+        <f t="shared" si="0"/>
+        <v>2.04</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="24">
+        <v>3</v>
+      </c>
+      <c r="H9" s="25">
+        <v>0.37</v>
+      </c>
+      <c r="I9" s="26">
+        <f t="shared" si="0"/>
+        <v>1.1099999999999999</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10" s="24">
+        <v>69</v>
+      </c>
+      <c r="H10" s="26">
+        <v>0.192</v>
+      </c>
+      <c r="I10" s="26">
+        <f t="shared" si="0"/>
+        <v>13.248000000000001</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="G11" s="24">
+        <v>9</v>
+      </c>
+      <c r="H11" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="I11" s="26">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="G12" s="24">
+        <v>12</v>
+      </c>
+      <c r="H12" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="26">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="G13" s="24">
+        <v>15</v>
+      </c>
+      <c r="H13" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="26">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="J13" s="28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="G14" s="24">
+        <v>36</v>
+      </c>
+      <c r="H14" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="26">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="G15" s="24">
+        <v>33</v>
+      </c>
+      <c r="H15" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="26">
+        <f t="shared" si="0"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="G16" s="24">
+        <v>4</v>
+      </c>
+      <c r="H16" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="I16" s="26">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="G17" s="24">
+        <v>27</v>
+      </c>
+      <c r="H17" s="25">
+        <v>0.16</v>
+      </c>
+      <c r="I17" s="26">
+        <f t="shared" si="0"/>
+        <v>4.32</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="G18" s="31">
+        <v>1</v>
+      </c>
+      <c r="H18" s="32">
+        <v>22.16</v>
+      </c>
+      <c r="I18" s="33">
+        <f t="shared" ref="I18:I68" si="1">G18*H18</f>
+        <v>22.16</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="G19" s="31">
+        <v>1</v>
+      </c>
+      <c r="H19" s="32">
+        <v>42.86</v>
+      </c>
+      <c r="I19" s="33">
+        <f t="shared" si="1"/>
+        <v>42.86</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="30" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="G20" s="31">
+        <v>1</v>
+      </c>
+      <c r="H20" s="32">
+        <v>20.95</v>
+      </c>
+      <c r="I20" s="33">
+        <f t="shared" si="1"/>
+        <v>20.95</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="E21" s="31"/>
+      <c r="F21" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="G21" s="31">
+        <v>2</v>
+      </c>
+      <c r="H21" s="32">
+        <v>0.21</v>
+      </c>
+      <c r="I21" s="33">
+        <f t="shared" si="1"/>
+        <v>0.42</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="E22" s="31"/>
+      <c r="F22" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="G22" s="31">
+        <v>2</v>
+      </c>
+      <c r="H22" s="32">
+        <v>0.43</v>
+      </c>
+      <c r="I22" s="33">
+        <f t="shared" si="1"/>
+        <v>0.86</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="E23" s="31"/>
+      <c r="F23" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="G23" s="31">
+        <v>2</v>
+      </c>
+      <c r="H23" s="32">
+        <v>0.43</v>
+      </c>
+      <c r="I23" s="33">
+        <f t="shared" si="1"/>
+        <v>0.86</v>
+      </c>
+      <c r="J23" s="34" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="E24" s="31"/>
+      <c r="F24" s="30" t="s">
+        <v>293</v>
+      </c>
+      <c r="G24" s="31">
+        <v>2</v>
+      </c>
+      <c r="H24" s="32">
+        <v>0.46</v>
+      </c>
+      <c r="I24" s="33">
+        <f t="shared" si="1"/>
+        <v>0.92</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="30"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="30"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="30"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="30"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="30"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="30"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="30"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="30"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="30"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="30"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" s="30"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="30"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="30"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="30"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="30"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="30"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="30"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="30"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="30"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="30"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="30"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="30"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="30"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="30"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="30"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="30"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="30"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="30"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="30"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="30"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="30"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="30"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I46" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I47" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I48" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I50" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I51" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I53" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I54" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I55" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I56" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I57" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I58" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I59" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I60" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I61" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I62" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I63" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I64" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I65" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I66" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I67" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I68" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I69" s="14">
+        <f t="shared" ref="I69:I102" si="2">G69*H69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I70" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I71" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I72" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I73" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I74" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I75" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I76" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I77" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I78" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I79" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I80" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I81" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I82" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I83" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I84" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I85" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I86" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I87" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I88" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I89" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I90" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I91" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I92" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I93" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I94" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I95" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I96" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I97" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I98" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I99" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I100" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I101" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I102" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{BFA2456D-8F7E-43CC-B2B0-D56DCE4C2C31}"/>
+    <hyperlink ref="J7" r:id="rId2" xr:uid="{48C9F0B2-72F5-49B6-BC70-9A5F80429FBC}"/>
+    <hyperlink ref="J13" r:id="rId3" xr:uid="{958BA2D2-DF00-4C15-AC6A-260F6CFD739A}"/>
+    <hyperlink ref="J24" r:id="rId4" xr:uid="{8959819C-F0D6-45AD-9BFA-8D120E1736F4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>